<commit_message>
Revert "Merge branch 'master' of https://github.com/FunabikiKeisuke/Hack-U"
This reverts commit dd6c14ca3cae2fc60eadc4612d929baaf032eec0, reversing
changes made to 657f2d6ca0f58e3cf99e196a608f2cb000b45b6f.
</commit_message>
<xml_diff>
--- a/素材/DB.xlsx
+++ b/素材/DB.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bicke\Documents\Hack-U\素材\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bicke\Documents\GitHub\Hack-U\素材\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1FD93C-85F2-429F-AE96-26B89C744D58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EB17BD-1496-4406-BC05-A5B4AF2D41AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7020" xr2:uid="{8A99A910-A21C-4608-B33E-0D2B138863BB}"/>
   </bookViews>
@@ -70,6 +70,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>ニックネーム</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>email</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -166,13 +170,6 @@
     </rPh>
     <rPh sb="3" eb="4">
       <t>ジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>氏名</t>
-    <rPh sb="0" eb="2">
-      <t>シメイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -550,7 +547,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -586,54 +583,54 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -680,46 +677,46 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Revert "Merge branch 'master' of https://github.com/FunabikiKeisuke/Hack-U""
This reverts commit d6cc9ba269d7e03ee68a0e23669b6bfc7c307b26.
</commit_message>
<xml_diff>
--- a/素材/DB.xlsx
+++ b/素材/DB.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bicke\Documents\GitHub\Hack-U\素材\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bicke\Documents\Hack-U\素材\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EB17BD-1496-4406-BC05-A5B4AF2D41AA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE1FD93C-85F2-429F-AE96-26B89C744D58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7020" xr2:uid="{8A99A910-A21C-4608-B33E-0D2B138863BB}"/>
   </bookViews>
@@ -70,10 +70,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>ニックネーム</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>email</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -170,6 +166,13 @@
     </rPh>
     <rPh sb="3" eb="4">
       <t>ジ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>氏名</t>
+    <rPh sb="0" eb="2">
+      <t>シメイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -547,7 +550,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.45"/>
@@ -583,54 +586,54 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
         <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -677,46 +680,46 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" t="s">
         <v>20</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
       <c r="C5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
       <c r="C6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>